<commit_message>
add cache for better UX
</commit_message>
<xml_diff>
--- a/output/Output Data Structure.xlsx
+++ b/output/Output Data Structure.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,30 +471,25 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>AVG NUMBER OF WORDS PER SENTENCE</t>
+          <t>COMPLEX WORD COUNT</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>COMPLEX WORD COUNT</t>
+          <t>WORD COUNT</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>WORD COUNT</t>
+          <t>SYLLABLE PER WORD</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>SYLLABLE PER WORD</t>
+          <t>PERSONAL PRONOUNS</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>PERSONAL PRONOUNS</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>AVG WORD LENGTH</t>
         </is>
@@ -525,21 +520,18 @@
         <v>6.92</v>
       </c>
       <c r="H2" t="n">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="I2" t="n">
-        <v>41</v>
+        <v>136</v>
       </c>
       <c r="J2" t="n">
-        <v>136</v>
+        <v>2.169</v>
       </c>
       <c r="K2" t="n">
-        <v>2.169</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" t="n">
         <v>6.632</v>
       </c>
     </row>
@@ -568,21 +560,18 @@
         <v>3.482</v>
       </c>
       <c r="H3" t="n">
-        <v>8.5</v>
+        <v>14</v>
       </c>
       <c r="I3" t="n">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="J3" t="n">
-        <v>68</v>
+        <v>2.015</v>
       </c>
       <c r="K3" t="n">
-        <v>2.015</v>
+        <v>4</v>
       </c>
       <c r="L3" t="n">
-        <v>4</v>
-      </c>
-      <c r="M3" t="n">
         <v>6.206</v>
       </c>
     </row>
@@ -611,21 +600,18 @@
         <v>6.168</v>
       </c>
       <c r="H4" t="n">
-        <v>15</v>
+        <v>673</v>
       </c>
       <c r="I4" t="n">
-        <v>673</v>
+        <v>1605</v>
       </c>
       <c r="J4" t="n">
-        <v>1605</v>
+        <v>2.414</v>
       </c>
       <c r="K4" t="n">
-        <v>2.414</v>
+        <v>1</v>
       </c>
       <c r="L4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M4" t="n">
         <v>7.128</v>
       </c>
     </row>

</xml_diff>

<commit_message>
resolved pdf charts issue
</commit_message>
<xml_diff>
--- a/output/Output Data Structure.xlsx
+++ b/output/Output Data Structure.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,82 +497,122 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://insights.blackcoffer.com/ai-and-ml-based-youtube-analytics-and-content-creation-tool-for-optimizing-subscriber-engagement-and-content-strategy/</t>
+          <t>https://realpython.com/tutorials/web-dev/</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-0.049</v>
+        <v>0.278</v>
       </c>
       <c r="D2" t="n">
-        <v>0.352</v>
+        <v>0.57</v>
       </c>
       <c r="E2" t="n">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F2" t="n">
-        <v>0.274</v>
+        <v>0.301</v>
       </c>
       <c r="G2" t="n">
-        <v>12.51</v>
+        <v>6.92</v>
       </c>
       <c r="H2" t="n">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="I2" t="n">
-        <v>186</v>
+        <v>136</v>
       </c>
       <c r="J2" t="n">
-        <v>2.027</v>
+        <v>2.169</v>
       </c>
       <c r="K2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>6.382</v>
+        <v>6.632</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://insights.blackcoffer.com/enhancing-front-end-features-and-functionality-for-improved-user-experience-and-dashboard-accuracy-in-partner-hospital-application/</t>
+          <t>https://python.land/introduction-to-python</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.16</v>
+        <v>0.19</v>
       </c>
       <c r="D3" t="n">
-        <v>0.445</v>
+        <v>0.47</v>
       </c>
       <c r="E3" t="n">
-        <v>13.167</v>
+        <v>8.5</v>
       </c>
       <c r="F3" t="n">
-        <v>0.278</v>
+        <v>0.206</v>
       </c>
       <c r="G3" t="n">
-        <v>5.378</v>
+        <v>3.482</v>
       </c>
       <c r="H3" t="n">
-        <v>132</v>
+        <v>14</v>
       </c>
       <c r="I3" t="n">
-        <v>474</v>
+        <v>68</v>
       </c>
       <c r="J3" t="n">
-        <v>2.093</v>
+        <v>2.015</v>
       </c>
       <c r="K3" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="L3" t="n">
-        <v>6.308</v>
+        <v>6.206</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>103</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://en.wikipedia.org/wiki/Natural_language_processing</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.429</v>
+      </c>
+      <c r="E4" t="n">
+        <v>15</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.419</v>
+      </c>
+      <c r="G4" t="n">
+        <v>6.168</v>
+      </c>
+      <c r="H4" t="n">
+        <v>673</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1605</v>
+      </c>
+      <c r="J4" t="n">
+        <v>2.414</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" t="n">
+        <v>7.128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added def for delete older pdf
</commit_message>
<xml_diff>
--- a/output/Output Data Structure.xlsx
+++ b/output/Output Data Structure.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,122 +497,82 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://realpython.com/tutorials/web-dev/</t>
+          <t>https://insights.blackcoffer.com/ai-and-ml-based-youtube-analytics-and-content-creation-tool-for-optimizing-subscriber-engagement-and-content-strategy/</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.278</v>
+        <v>-0.033</v>
       </c>
       <c r="D2" t="n">
-        <v>0.57</v>
+        <v>0.311</v>
       </c>
       <c r="E2" t="n">
-        <v>17</v>
+        <v>18.667</v>
       </c>
       <c r="F2" t="n">
-        <v>0.301</v>
+        <v>0.357</v>
       </c>
       <c r="G2" t="n">
-        <v>6.92</v>
+        <v>7.61</v>
       </c>
       <c r="H2" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I2" t="n">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="J2" t="n">
-        <v>2.169</v>
+        <v>2.188</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" t="n">
-        <v>6.632</v>
+        <v>6.857</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://python.land/introduction-to-python</t>
+          <t>https://insights.blackcoffer.com/enhancing-front-end-features-and-functionality-for-improved-user-experience-and-dashboard-accuracy-in-partner-hospital-application/</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.19</v>
+        <v>0.16</v>
       </c>
       <c r="D3" t="n">
-        <v>0.47</v>
+        <v>0.445</v>
       </c>
       <c r="E3" t="n">
-        <v>8.5</v>
+        <v>13.167</v>
       </c>
       <c r="F3" t="n">
-        <v>0.206</v>
+        <v>0.278</v>
       </c>
       <c r="G3" t="n">
-        <v>3.482</v>
+        <v>5.378</v>
       </c>
       <c r="H3" t="n">
-        <v>14</v>
+        <v>132</v>
       </c>
       <c r="I3" t="n">
-        <v>68</v>
+        <v>474</v>
       </c>
       <c r="J3" t="n">
-        <v>2.015</v>
+        <v>2.093</v>
       </c>
       <c r="K3" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="L3" t="n">
-        <v>6.206</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>103</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>https://en.wikipedia.org/wiki/Natural_language_processing</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.429</v>
-      </c>
-      <c r="E4" t="n">
-        <v>15</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.419</v>
-      </c>
-      <c r="G4" t="n">
-        <v>6.168</v>
-      </c>
-      <c r="H4" t="n">
-        <v>673</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1605</v>
-      </c>
-      <c r="J4" t="n">
-        <v>2.414</v>
-      </c>
-      <c r="K4" t="n">
-        <v>1</v>
-      </c>
-      <c r="L4" t="n">
-        <v>7.128</v>
+        <v>6.308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added SS of app
</commit_message>
<xml_diff>
--- a/output/Output Data Structure.xlsx
+++ b/output/Output Data Structure.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,82 +497,122 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://insights.blackcoffer.com/ai-and-ml-based-youtube-analytics-and-content-creation-tool-for-optimizing-subscriber-engagement-and-content-strategy/</t>
+          <t>https://realpython.com/tutorials/web-dev/</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-0.033</v>
+        <v>0.278</v>
       </c>
       <c r="D2" t="n">
-        <v>0.311</v>
+        <v>0.57</v>
       </c>
       <c r="E2" t="n">
-        <v>18.667</v>
+        <v>17</v>
       </c>
       <c r="F2" t="n">
-        <v>0.357</v>
+        <v>0.301</v>
       </c>
       <c r="G2" t="n">
-        <v>7.61</v>
+        <v>6.92</v>
       </c>
       <c r="H2" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I2" t="n">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="J2" t="n">
-        <v>2.188</v>
+        <v>2.169</v>
       </c>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>6.857</v>
+        <v>6.632</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://insights.blackcoffer.com/enhancing-front-end-features-and-functionality-for-improved-user-experience-and-dashboard-accuracy-in-partner-hospital-application/</t>
+          <t>https://python.land/introduction-to-python</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.16</v>
+        <v>0.19</v>
       </c>
       <c r="D3" t="n">
-        <v>0.445</v>
+        <v>0.47</v>
       </c>
       <c r="E3" t="n">
-        <v>13.167</v>
+        <v>8.5</v>
       </c>
       <c r="F3" t="n">
-        <v>0.278</v>
+        <v>0.206</v>
       </c>
       <c r="G3" t="n">
-        <v>5.378</v>
+        <v>3.482</v>
       </c>
       <c r="H3" t="n">
-        <v>132</v>
+        <v>14</v>
       </c>
       <c r="I3" t="n">
-        <v>474</v>
+        <v>68</v>
       </c>
       <c r="J3" t="n">
-        <v>2.093</v>
+        <v>2.015</v>
       </c>
       <c r="K3" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="L3" t="n">
-        <v>6.308</v>
+        <v>6.206</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>103</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://en.wikipedia.org/wiki/Natural_language_processing</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.429</v>
+      </c>
+      <c r="E4" t="n">
+        <v>15</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.419</v>
+      </c>
+      <c r="G4" t="n">
+        <v>6.168</v>
+      </c>
+      <c r="H4" t="n">
+        <v>673</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1605</v>
+      </c>
+      <c r="J4" t="n">
+        <v>2.414</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" t="n">
+        <v>7.128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>